<commit_message>
feat: update MapLibreMap component to use external URLs for tile sources
</commit_message>
<xml_diff>
--- a/README_2.xlsx
+++ b/README_2.xlsx
@@ -197,7 +197,17 @@
     <t xml:space="preserve">GPKG</t>
   </si>
   <si>
-    <t xml:space="preserve">Vehicle types, Daily values</t>
+    <t xml:space="preserve">PW - Passenger Car (Personenwagen): Refers to personal vehicles used for individual transport.
+LI - Delivery Vehicle (Lieferwagen): Vehicles primarily used for delivery and goods transportation.
+LW - Lorry (Lastwagen): Refers to heavy-duty trucks and similar larger goods vehicles.
+LZ - Articulated Lorry (Lastzüge): Semi-trailers or other articulated vehicles used for freight transport.
+DWV - Average Workday Traffic (Durchschnittlicher Werktagverkehr): The average number of vehicles passing a point on a typical workday.
+DTV - Average Daily Traffic (Durchschnittlicher Tagesverkehr): The average vehicle traffic per day, across all days of the week.
+MSP - Morning Peak Hour (Morgenspitze): The morning rush hour, usually between 7 AM and 8 AM, indicating peak traffic levels.
+ASP - Evening Peak Hour (Abendspitze): The evening rush hour, typically between 5 PM and 6 PM, indicating peak traffic levels.
+NPVM - National Passenger Traffic Model: A model for analyzing and forecasting passenger traffic.
+AMG - Aggregated Method for Freight Traffic (Aggregierte Methode Güterverkehr): A method used for calculating and analyzing freight traffic data.
+</t>
   </si>
   <si>
     <t xml:space="preserve">Load (vehicles) on the Swiss road network (passengers and freight) 2050</t>
@@ -348,7 +358,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +393,13 @@
       <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -440,7 +457,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -463,6 +480,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -712,7 +733,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,7 +945,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -955,7 +976,7 @@
       <c r="J6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1095,7 +1116,7 @@
       <c r="J10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L10" s="5" t="s">

</xml_diff>